<commit_message>
Added second version details with review comments
</commit_message>
<xml_diff>
--- a/TPDS/experiments/ osp_sq_max_final_18_10_2022.xlsx
+++ b/TPDS/experiments/ osp_sq_max_final_18_10_2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MyDocuments/Techinical Documents/Masters/Thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiranjeb/alphaz-user-docker/workspace/bpmax_cpu/TPDS/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1AC035-7B47-0F42-A160-18FC39A6668F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4781D824-9B6D-A344-A927-5DAF6D62F5D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="920" windowWidth="35220" windowHeight="19640" activeTab="1" xr2:uid="{2250EDDF-9FCA-1048-8588-54EA16156B4A}"/>
+    <workbookView xWindow="5000" yWindow="920" windowWidth="35220" windowHeight="19640" activeTab="3" xr2:uid="{2250EDDF-9FCA-1048-8588-54EA16156B4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Coffee Lake Best Tile" sheetId="9" r:id="rId1"/>
@@ -971,6 +971,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -981,6 +992,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1010,20 +1024,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -21691,16 +21691,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>67056</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>194056</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22309,7 +22309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD6DBB7-476F-4E4B-BD60-4062C60819F1}">
   <dimension ref="A6:P38"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
@@ -22320,44 +22320,44 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49" t="s">
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49" t="s">
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49" t="s">
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49" t="s">
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="O6" s="49"/>
-      <c r="P6" s="49"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
     </row>
     <row r="7" spans="1:16" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:16" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
@@ -22816,18 +22816,18 @@
     <row r="22" spans="1:16" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
     <row r="23" spans="1:16" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
     <row r="24" spans="1:16" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
     </row>
     <row r="25" spans="1:16" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="34" t="s">
@@ -23221,18 +23221,18 @@
     </row>
     <row r="31" spans="1:16" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.15"/>
     <row r="32" spans="1:16" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
     </row>
     <row r="33" spans="1:16" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="34" t="s">
@@ -24579,51 +24579,51 @@
     <row r="16" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F16" s="23"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="60" t="s">
+      <c r="H16" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60" t="s">
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="66"/>
+      <c r="O16" s="66"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="60"/>
-      <c r="U16" s="60" t="s">
+      <c r="R16" s="66"/>
+      <c r="S16" s="66"/>
+      <c r="T16" s="66"/>
+      <c r="U16" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="V16" s="60"/>
-      <c r="W16" s="60"/>
-      <c r="X16" s="60"/>
-      <c r="Y16" s="60"/>
-      <c r="Z16" s="60"/>
-      <c r="AA16" s="60"/>
-      <c r="AB16" s="60"/>
-      <c r="AC16" s="60"/>
-      <c r="AD16" s="60"/>
-      <c r="AE16" s="60"/>
-      <c r="AF16" s="60"/>
-      <c r="AG16" s="60"/>
-      <c r="AH16" s="60"/>
-      <c r="AI16" s="60"/>
-      <c r="AJ16" s="60"/>
-      <c r="AK16" s="60" t="s">
+      <c r="V16" s="66"/>
+      <c r="W16" s="66"/>
+      <c r="X16" s="66"/>
+      <c r="Y16" s="66"/>
+      <c r="Z16" s="66"/>
+      <c r="AA16" s="66"/>
+      <c r="AB16" s="66"/>
+      <c r="AC16" s="66"/>
+      <c r="AD16" s="66"/>
+      <c r="AE16" s="66"/>
+      <c r="AF16" s="66"/>
+      <c r="AG16" s="66"/>
+      <c r="AH16" s="66"/>
+      <c r="AI16" s="66"/>
+      <c r="AJ16" s="66"/>
+      <c r="AK16" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="AL16" s="60"/>
-      <c r="AM16" s="60"/>
-      <c r="AN16" s="60"/>
-      <c r="AO16" s="60"/>
-      <c r="AP16" s="60"/>
-      <c r="AQ16" s="60"/>
-      <c r="AR16" s="60"/>
+      <c r="AL16" s="66"/>
+      <c r="AM16" s="66"/>
+      <c r="AN16" s="66"/>
+      <c r="AO16" s="66"/>
+      <c r="AP16" s="66"/>
+      <c r="AQ16" s="66"/>
+      <c r="AR16" s="66"/>
     </row>
     <row r="17" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
@@ -25105,57 +25105,57 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:27" ht="28" x14ac:dyDescent="0.3">
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51" t="s">
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51" t="s">
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51" t="s">
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="50" t="s">
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="55"/>
+      <c r="V3" s="55"/>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="53"/>
+      <c r="R4" s="53"/>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.15">
       <c r="C5" s="9" t="s">
@@ -25731,25 +25731,25 @@
       <c r="F14" s="15"/>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.15">
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="48"/>
-      <c r="Q21" s="48"/>
-      <c r="R21" s="48"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="53"/>
+      <c r="O21" s="53"/>
+      <c r="P21" s="53"/>
+      <c r="Q21" s="53"/>
+      <c r="R21" s="53"/>
     </row>
     <row r="22" spans="2:22" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B22" s="18" t="s">
@@ -26177,25 +26177,25 @@
       </c>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.15">
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="48"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="48"/>
-      <c r="O29" s="48"/>
-      <c r="P29" s="48"/>
-      <c r="Q29" s="48"/>
-      <c r="R29" s="48"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="53"/>
+      <c r="P29" s="53"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="53"/>
     </row>
     <row r="31" spans="2:22" s="18" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B31" s="17" t="s">
@@ -27519,7 +27519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC38A14-BCC4-4E43-B6A9-5F777B55E1F3}">
   <dimension ref="A3:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -27535,38 +27535,38 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:17" ht="28" x14ac:dyDescent="0.3">
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
       <c r="D3" s="20"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
       <c r="G3" s="20"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
       <c r="J3" s="20"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
       <c r="M3" s="20"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
       <c r="M4" s="19"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.15">
@@ -27994,21 +27994,21 @@
       <c r="D14" s="15"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
@@ -28341,21 +28341,21 @@
       <c r="Q26" s="18"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="48"/>
-      <c r="M29" s="48"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="53"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A31" s="17" t="s">
@@ -28641,8 +28641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B5BF7B-DDC6-B649-B4C2-E40E1B80C594}">
   <dimension ref="B16:T61"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="T44" sqref="T44"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29945,8 +29945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4172040F-BF89-DB4B-89B8-98400F3218B3}">
   <dimension ref="A4:X55"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30004,14 +30004,14 @@
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
       <c r="H8" s="32"/>
-      <c r="S8" s="61" t="s">
+      <c r="S8" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="T8" s="61"/>
-      <c r="U8" s="61"/>
-      <c r="V8" s="61"/>
-      <c r="W8" s="61"/>
-      <c r="X8" s="61"/>
+      <c r="T8" s="57"/>
+      <c r="U8" s="57"/>
+      <c r="V8" s="57"/>
+      <c r="W8" s="57"/>
+      <c r="X8" s="57"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="32"/>
@@ -30022,20 +30022,20 @@
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
       <c r="H9" s="32"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="63" t="s">
+      <c r="S9" s="48"/>
+      <c r="T9" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="U9" s="63" t="s">
+      <c r="U9" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="V9" s="63" t="s">
+      <c r="V9" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="W9" s="64" t="s">
+      <c r="W9" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="X9" s="64" t="s">
+      <c r="X9" s="50" t="s">
         <v>176</v>
       </c>
     </row>
@@ -30048,22 +30048,22 @@
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
-      <c r="S10" s="65" t="s">
+      <c r="S10" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="T10" s="66">
+      <c r="T10" s="52">
         <v>15.61</v>
       </c>
-      <c r="U10" s="66">
+      <c r="U10" s="52">
         <v>15.62</v>
       </c>
-      <c r="V10" s="66">
+      <c r="V10" s="52">
         <v>15.65</v>
       </c>
-      <c r="W10" s="66">
+      <c r="W10" s="52">
         <v>15.58</v>
       </c>
-      <c r="X10" s="66">
+      <c r="X10" s="52">
         <v>15.6</v>
       </c>
     </row>
@@ -30076,14 +30076,14 @@
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
       <c r="H11" s="32"/>
-      <c r="S11" s="65" t="s">
+      <c r="S11" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="T11" s="66"/>
-      <c r="U11" s="66"/>
-      <c r="V11" s="66"/>
-      <c r="W11" s="66"/>
-      <c r="X11" s="66"/>
+      <c r="T11" s="52"/>
+      <c r="U11" s="52"/>
+      <c r="V11" s="52"/>
+      <c r="W11" s="52"/>
+      <c r="X11" s="52"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="32"/>
@@ -30094,14 +30094,14 @@
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
       <c r="H12" s="32"/>
-      <c r="S12" s="65" t="s">
+      <c r="S12" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="T12" s="66"/>
-      <c r="U12" s="66"/>
-      <c r="V12" s="66"/>
-      <c r="W12" s="66"/>
-      <c r="X12" s="66"/>
+      <c r="T12" s="52"/>
+      <c r="U12" s="52"/>
+      <c r="V12" s="52"/>
+      <c r="W12" s="52"/>
+      <c r="X12" s="52"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="32"/>
@@ -30112,14 +30112,14 @@
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
       <c r="H13" s="32"/>
-      <c r="S13" s="65" t="s">
+      <c r="S13" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="T13" s="66"/>
-      <c r="U13" s="66"/>
-      <c r="V13" s="66"/>
-      <c r="W13" s="66"/>
-      <c r="X13" s="66"/>
+      <c r="T13" s="52"/>
+      <c r="U13" s="52"/>
+      <c r="V13" s="52"/>
+      <c r="W13" s="52"/>
+      <c r="X13" s="52"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="32"/>
@@ -30130,14 +30130,14 @@
       <c r="F14" s="32"/>
       <c r="G14" s="32"/>
       <c r="H14" s="32"/>
-      <c r="S14" s="65" t="s">
+      <c r="S14" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="T14" s="66"/>
-      <c r="U14" s="66"/>
-      <c r="V14" s="66"/>
-      <c r="W14" s="66"/>
-      <c r="X14" s="66"/>
+      <c r="T14" s="52"/>
+      <c r="U14" s="52"/>
+      <c r="V14" s="52"/>
+      <c r="W14" s="52"/>
+      <c r="X14" s="52"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="32"/>
@@ -30148,14 +30148,14 @@
       <c r="F15" s="32"/>
       <c r="G15" s="32"/>
       <c r="H15" s="32"/>
-      <c r="S15" s="65" t="s">
+      <c r="S15" s="51" t="s">
         <v>177</v>
       </c>
-      <c r="T15" s="66"/>
-      <c r="U15" s="66"/>
-      <c r="V15" s="66"/>
-      <c r="W15" s="66"/>
-      <c r="X15" s="66"/>
+      <c r="T15" s="52"/>
+      <c r="U15" s="52"/>
+      <c r="V15" s="52"/>
+      <c r="W15" s="52"/>
+      <c r="X15" s="52"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="32"/>
@@ -30166,12 +30166,12 @@
       <c r="F16" s="32"/>
       <c r="G16" s="32"/>
       <c r="H16" s="32"/>
-      <c r="S16" s="62"/>
-      <c r="T16" s="66"/>
-      <c r="U16" s="66"/>
-      <c r="V16" s="66"/>
-      <c r="W16" s="66"/>
-      <c r="X16" s="66"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="52"/>
+      <c r="U16" s="52"/>
+      <c r="V16" s="52"/>
+      <c r="W16" s="52"/>
+      <c r="X16" s="52"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="32"/>
@@ -30210,14 +30210,14 @@
       </c>
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
-      <c r="S19" s="61" t="s">
+      <c r="S19" s="57" t="s">
         <v>178</v>
       </c>
-      <c r="T19" s="61"/>
-      <c r="U19" s="61"/>
-      <c r="V19" s="61"/>
-      <c r="W19" s="61"/>
-      <c r="X19" s="61"/>
+      <c r="T19" s="57"/>
+      <c r="U19" s="57"/>
+      <c r="V19" s="57"/>
+      <c r="W19" s="57"/>
+      <c r="X19" s="57"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="32"/>
@@ -30238,20 +30238,20 @@
       </c>
       <c r="G20" s="32"/>
       <c r="H20" s="32"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="63" t="s">
+      <c r="S20" s="48"/>
+      <c r="T20" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="U20" s="63" t="s">
+      <c r="U20" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="V20" s="63" t="s">
+      <c r="V20" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="W20" s="64" t="s">
+      <c r="W20" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="X20" s="64" t="s">
+      <c r="X20" s="50" t="s">
         <v>176</v>
       </c>
     </row>
@@ -30268,14 +30268,14 @@
       <c r="F21" s="32"/>
       <c r="G21" s="32"/>
       <c r="H21" s="32"/>
-      <c r="S21" s="65" t="s">
+      <c r="S21" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="T21" s="66"/>
-      <c r="U21" s="66"/>
-      <c r="V21" s="66"/>
-      <c r="W21" s="66"/>
-      <c r="X21" s="66"/>
+      <c r="T21" s="52"/>
+      <c r="U21" s="52"/>
+      <c r="V21" s="52"/>
+      <c r="W21" s="52"/>
+      <c r="X21" s="52"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="32"/>
@@ -30290,14 +30290,14 @@
       <c r="F22" s="32"/>
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
-      <c r="S22" s="65" t="s">
+      <c r="S22" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="T22" s="66"/>
-      <c r="U22" s="66"/>
-      <c r="V22" s="66"/>
-      <c r="W22" s="66"/>
-      <c r="X22" s="66"/>
+      <c r="T22" s="52"/>
+      <c r="U22" s="52"/>
+      <c r="V22" s="52"/>
+      <c r="W22" s="52"/>
+      <c r="X22" s="52"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="32"/>
@@ -30310,14 +30310,14 @@
       <c r="F23" s="32"/>
       <c r="G23" s="32"/>
       <c r="H23" s="32"/>
-      <c r="S23" s="65" t="s">
+      <c r="S23" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="T23" s="66"/>
-      <c r="U23" s="66"/>
-      <c r="V23" s="66"/>
-      <c r="W23" s="66"/>
-      <c r="X23" s="66"/>
+      <c r="T23" s="52"/>
+      <c r="U23" s="52"/>
+      <c r="V23" s="52"/>
+      <c r="W23" s="52"/>
+      <c r="X23" s="52"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="32"/>
@@ -30328,14 +30328,14 @@
       <c r="F24" s="32"/>
       <c r="G24" s="32"/>
       <c r="H24" s="32"/>
-      <c r="S24" s="65" t="s">
+      <c r="S24" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="T24" s="66"/>
-      <c r="U24" s="66"/>
-      <c r="V24" s="66"/>
-      <c r="W24" s="66"/>
-      <c r="X24" s="66"/>
+      <c r="T24" s="52"/>
+      <c r="U24" s="52"/>
+      <c r="V24" s="52"/>
+      <c r="W24" s="52"/>
+      <c r="X24" s="52"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="32"/>
@@ -30346,14 +30346,14 @@
       <c r="F25" s="32"/>
       <c r="G25" s="32"/>
       <c r="H25" s="32"/>
-      <c r="S25" s="65" t="s">
+      <c r="S25" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="T25" s="66"/>
-      <c r="U25" s="66"/>
-      <c r="V25" s="66"/>
-      <c r="W25" s="66"/>
-      <c r="X25" s="66"/>
+      <c r="T25" s="52"/>
+      <c r="U25" s="52"/>
+      <c r="V25" s="52"/>
+      <c r="W25" s="52"/>
+      <c r="X25" s="52"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="32"/>
@@ -30364,14 +30364,14 @@
       <c r="F26" s="32"/>
       <c r="G26" s="32"/>
       <c r="H26" s="32"/>
-      <c r="S26" s="65" t="s">
+      <c r="S26" s="51" t="s">
         <v>177</v>
       </c>
-      <c r="T26" s="66"/>
-      <c r="U26" s="66"/>
-      <c r="V26" s="66"/>
-      <c r="W26" s="66"/>
-      <c r="X26" s="66"/>
+      <c r="T26" s="52"/>
+      <c r="U26" s="52"/>
+      <c r="V26" s="52"/>
+      <c r="W26" s="52"/>
+      <c r="X26" s="52"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="32"/>
@@ -30382,12 +30382,12 @@
       <c r="F27" s="32"/>
       <c r="G27" s="32"/>
       <c r="H27" s="32"/>
-      <c r="S27" s="62"/>
-      <c r="T27" s="66"/>
-      <c r="U27" s="66"/>
-      <c r="V27" s="66"/>
-      <c r="W27" s="66"/>
-      <c r="X27" s="66"/>
+      <c r="S27" s="48"/>
+      <c r="T27" s="52"/>
+      <c r="U27" s="52"/>
+      <c r="V27" s="52"/>
+      <c r="W27" s="52"/>
+      <c r="X27" s="52"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="32"/>
@@ -30512,14 +30512,14 @@
       <c r="F36" s="32"/>
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
-      <c r="S36" s="61" t="s">
+      <c r="S36" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="T36" s="61"/>
-      <c r="U36" s="61"/>
-      <c r="V36" s="61"/>
-      <c r="W36" s="61"/>
-      <c r="X36" s="61"/>
+      <c r="T36" s="57"/>
+      <c r="U36" s="57"/>
+      <c r="V36" s="57"/>
+      <c r="W36" s="57"/>
+      <c r="X36" s="57"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="32"/>
@@ -30530,20 +30530,20 @@
       <c r="F37" s="32"/>
       <c r="G37" s="32"/>
       <c r="H37" s="32"/>
-      <c r="S37" s="62"/>
-      <c r="T37" s="63" t="s">
+      <c r="S37" s="48"/>
+      <c r="T37" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="U37" s="63" t="s">
+      <c r="U37" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="V37" s="63" t="s">
+      <c r="V37" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="W37" s="64" t="s">
+      <c r="W37" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="X37" s="64" t="s">
+      <c r="X37" s="50" t="s">
         <v>176</v>
       </c>
     </row>
@@ -30556,14 +30556,14 @@
       <c r="F38" s="32"/>
       <c r="G38" s="32"/>
       <c r="H38" s="32"/>
-      <c r="S38" s="65" t="s">
+      <c r="S38" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="T38" s="66"/>
-      <c r="U38" s="66"/>
-      <c r="V38" s="66"/>
-      <c r="W38" s="66"/>
-      <c r="X38" s="66"/>
+      <c r="T38" s="52"/>
+      <c r="U38" s="52"/>
+      <c r="V38" s="52"/>
+      <c r="W38" s="52"/>
+      <c r="X38" s="52"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="32"/>
@@ -30574,14 +30574,14 @@
       <c r="F39" s="32"/>
       <c r="G39" s="32"/>
       <c r="H39" s="32"/>
-      <c r="S39" s="65" t="s">
+      <c r="S39" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="T39" s="66"/>
-      <c r="U39" s="66"/>
-      <c r="V39" s="66"/>
-      <c r="W39" s="66"/>
-      <c r="X39" s="66"/>
+      <c r="T39" s="52"/>
+      <c r="U39" s="52"/>
+      <c r="V39" s="52"/>
+      <c r="W39" s="52"/>
+      <c r="X39" s="52"/>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="32"/>
@@ -30592,14 +30592,14 @@
       <c r="F40" s="32"/>
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
-      <c r="S40" s="65" t="s">
+      <c r="S40" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="T40" s="66"/>
-      <c r="U40" s="66"/>
-      <c r="V40" s="66"/>
-      <c r="W40" s="66"/>
-      <c r="X40" s="66"/>
+      <c r="T40" s="52"/>
+      <c r="U40" s="52"/>
+      <c r="V40" s="52"/>
+      <c r="W40" s="52"/>
+      <c r="X40" s="52"/>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="32"/>
@@ -30622,14 +30622,14 @@
       <c r="H41" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S41" s="65" t="s">
+      <c r="S41" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="T41" s="66"/>
-      <c r="U41" s="66"/>
-      <c r="V41" s="66"/>
-      <c r="W41" s="66"/>
-      <c r="X41" s="66"/>
+      <c r="T41" s="52"/>
+      <c r="U41" s="52"/>
+      <c r="V41" s="52"/>
+      <c r="W41" s="52"/>
+      <c r="X41" s="52"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="32"/>
@@ -30654,14 +30654,14 @@
       <c r="H42" s="32">
         <v>10244</v>
       </c>
-      <c r="S42" s="65" t="s">
+      <c r="S42" s="51" t="s">
         <v>73</v>
       </c>
       <c r="T42" s="33"/>
-      <c r="U42" s="66"/>
-      <c r="V42" s="66"/>
-      <c r="W42" s="66"/>
-      <c r="X42" s="66"/>
+      <c r="U42" s="52"/>
+      <c r="V42" s="52"/>
+      <c r="W42" s="52"/>
+      <c r="X42" s="52"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="32"/>
@@ -30686,14 +30686,14 @@
       <c r="H43" s="32">
         <v>3544</v>
       </c>
-      <c r="S43" s="65" t="s">
+      <c r="S43" s="51" t="s">
         <v>177</v>
       </c>
       <c r="T43" s="33"/>
-      <c r="U43" s="66"/>
-      <c r="V43" s="66"/>
-      <c r="W43" s="66"/>
-      <c r="X43" s="66"/>
+      <c r="U43" s="52"/>
+      <c r="V43" s="52"/>
+      <c r="W43" s="52"/>
+      <c r="X43" s="52"/>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="32"/>
@@ -30718,12 +30718,12 @@
       <c r="H44" s="32">
         <v>6202</v>
       </c>
-      <c r="S44" s="62"/>
-      <c r="T44" s="66"/>
-      <c r="U44" s="66"/>
-      <c r="V44" s="66"/>
-      <c r="W44" s="66"/>
-      <c r="X44" s="66"/>
+      <c r="S44" s="48"/>
+      <c r="T44" s="52"/>
+      <c r="U44" s="52"/>
+      <c r="V44" s="52"/>
+      <c r="W44" s="52"/>
+      <c r="X44" s="52"/>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="32"/>
@@ -30977,42 +30977,42 @@
   </cols>
   <sheetData>
     <row r="13" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="54"/>
-      <c r="R13" s="52" t="s">
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="60"/>
+      <c r="R13" s="58" t="s">
         <v>146</v>
       </c>
-      <c r="S13" s="53"/>
-      <c r="T13" s="53"/>
-      <c r="U13" s="53"/>
-      <c r="V13" s="53"/>
-      <c r="W13" s="53"/>
-      <c r="X13" s="53"/>
-      <c r="Y13" s="54"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="59"/>
+      <c r="U13" s="59"/>
+      <c r="V13" s="59"/>
+      <c r="W13" s="59"/>
+      <c r="X13" s="59"/>
+      <c r="Y13" s="60"/>
     </row>
     <row r="14" spans="3:25" x14ac:dyDescent="0.2">
-      <c r="C14" s="55"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="57"/>
-      <c r="R14" s="55"/>
-      <c r="S14" s="56"/>
-      <c r="T14" s="56"/>
-      <c r="U14" s="56"/>
-      <c r="V14" s="56"/>
-      <c r="W14" s="56"/>
-      <c r="X14" s="56"/>
-      <c r="Y14" s="57"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="63"/>
+      <c r="R14" s="61"/>
+      <c r="S14" s="62"/>
+      <c r="T14" s="62"/>
+      <c r="U14" s="62"/>
+      <c r="V14" s="62"/>
+      <c r="W14" s="62"/>
+      <c r="X14" s="62"/>
+      <c r="Y14" s="63"/>
     </row>
     <row r="15" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C15" s="45"/>
@@ -31302,75 +31302,75 @@
     </row>
     <row r="35" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B35" s="38"/>
-      <c r="C35" s="58" t="s">
+      <c r="C35" s="64" t="s">
         <v>149</v>
       </c>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
-      <c r="O35" s="58"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="58"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="64"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="64"/>
+      <c r="N35" s="64"/>
+      <c r="O35" s="64"/>
+      <c r="P35" s="64"/>
+      <c r="Q35" s="64"/>
       <c r="S35" s="38"/>
-      <c r="T35" s="58" t="s">
+      <c r="T35" s="64" t="s">
         <v>149</v>
       </c>
-      <c r="U35" s="58"/>
-      <c r="V35" s="58"/>
-      <c r="W35" s="58"/>
-      <c r="X35" s="58"/>
-      <c r="Y35" s="58"/>
-      <c r="Z35" s="58"/>
-      <c r="AA35" s="58"/>
-      <c r="AB35" s="58"/>
-      <c r="AC35" s="58"/>
-      <c r="AD35" s="58"/>
-      <c r="AE35" s="58"/>
-      <c r="AF35" s="58"/>
-      <c r="AG35" s="58"/>
-      <c r="AH35" s="58"/>
+      <c r="U35" s="64"/>
+      <c r="V35" s="64"/>
+      <c r="W35" s="64"/>
+      <c r="X35" s="64"/>
+      <c r="Y35" s="64"/>
+      <c r="Z35" s="64"/>
+      <c r="AA35" s="64"/>
+      <c r="AB35" s="64"/>
+      <c r="AC35" s="64"/>
+      <c r="AD35" s="64"/>
+      <c r="AE35" s="64"/>
+      <c r="AF35" s="64"/>
+      <c r="AG35" s="64"/>
+      <c r="AH35" s="64"/>
     </row>
     <row r="36" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B36" s="38"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="59"/>
-      <c r="K36" s="59"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="59"/>
-      <c r="N36" s="59"/>
-      <c r="O36" s="59"/>
-      <c r="P36" s="59"/>
-      <c r="Q36" s="59"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
+      <c r="K36" s="65"/>
+      <c r="L36" s="65"/>
+      <c r="M36" s="65"/>
+      <c r="N36" s="65"/>
+      <c r="O36" s="65"/>
+      <c r="P36" s="65"/>
+      <c r="Q36" s="65"/>
       <c r="S36" s="38"/>
-      <c r="T36" s="59"/>
-      <c r="U36" s="59"/>
-      <c r="V36" s="59"/>
-      <c r="W36" s="59"/>
-      <c r="X36" s="59"/>
-      <c r="Y36" s="59"/>
-      <c r="Z36" s="59"/>
-      <c r="AA36" s="59"/>
-      <c r="AB36" s="59"/>
-      <c r="AC36" s="59"/>
-      <c r="AD36" s="59"/>
-      <c r="AE36" s="59"/>
-      <c r="AF36" s="59"/>
-      <c r="AG36" s="59"/>
-      <c r="AH36" s="59"/>
+      <c r="T36" s="65"/>
+      <c r="U36" s="65"/>
+      <c r="V36" s="65"/>
+      <c r="W36" s="65"/>
+      <c r="X36" s="65"/>
+      <c r="Y36" s="65"/>
+      <c r="Z36" s="65"/>
+      <c r="AA36" s="65"/>
+      <c r="AB36" s="65"/>
+      <c r="AC36" s="65"/>
+      <c r="AD36" s="65"/>
+      <c r="AE36" s="65"/>
+      <c r="AF36" s="65"/>
+      <c r="AG36" s="65"/>
+      <c r="AH36" s="65"/>
     </row>
     <row r="37" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B37" s="38"/>

</xml_diff>